<commit_message>
TEXT ANALYSIS - working on text analysis
</commit_message>
<xml_diff>
--- a/FinalCorpus/mediaWordsCombinations.xlsx
+++ b/FinalCorpus/mediaWordsCombinations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\le_rap_francophone\Final Corpus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\le_rap_francophone\FinalCorpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9684A83E-36F9-4A52-B954-3FE4427511B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E113E8D-746E-4DD4-AE65-55A5CBC28509}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6C5CF591-679C-41E9-B03E-168F6DCB78C1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Social Media</t>
   </si>
@@ -169,6 +169,30 @@
   </si>
   <si>
     <t>Big Brother</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Radio Nova</t>
+  </si>
+  <si>
+    <t>France Inter</t>
+  </si>
+  <si>
+    <t>Journaux</t>
+  </si>
+  <si>
+    <t>Télé</t>
+  </si>
+  <si>
+    <t>France bleu</t>
+  </si>
+  <si>
+    <t>Le Monde</t>
+  </si>
+  <si>
+    <t>last.fm</t>
   </si>
 </sst>
 </file>
@@ -559,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E680BAF-B641-4CB2-A53E-D08889267538}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,9 +608,10 @@
     <col min="16" max="16" width="14.6328125" customWidth="1"/>
     <col min="17" max="17" width="16.36328125" customWidth="1"/>
     <col min="18" max="18" width="13.08984375" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -641,8 +666,17 @@
       <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -667,6 +701,9 @@
       <c r="J2" t="s">
         <v>32</v>
       </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
       <c r="M2" t="s">
         <v>33</v>
       </c>
@@ -679,8 +716,14 @@
       <c r="R2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -696,8 +739,11 @@
       <c r="P3" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -710,8 +756,11 @@
       <c r="P4" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -722,7 +771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -730,37 +779,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="P7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>